<commit_message>
updated the gift box
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACA5A57-9149-47FD-A56B-931A3D2FC202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FED75241-5C03-47B0-83A8-02014C9CFF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9916733-9D91-48E8-84F6-9F67B5547383}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -45,18 +45,86 @@
     <t>stockavailable</t>
   </si>
   <si>
-    <t>Product B3</t>
-  </si>
-  <si>
-    <t>Product A3</t>
+    <t>Sparklers</t>
+  </si>
+  <si>
+    <t>Flower Pots</t>
+  </si>
+  <si>
+    <t>Chakras (Ground Spinners)</t>
+  </si>
+  <si>
+    <t>Atom Bombs</t>
+  </si>
+  <si>
+    <t>Rocket Bombs</t>
+  </si>
+  <si>
+    <t>Zameen Chakkars</t>
+  </si>
+  <si>
+    <t>Lakshmi Bombs</t>
+  </si>
+  <si>
+    <t>Rassi Bombs</t>
+  </si>
+  <si>
+    <t>Pencil Sparklers</t>
+  </si>
+  <si>
+    <t>Bullet Bombs</t>
+  </si>
+  <si>
+    <t>Sky Shots</t>
+  </si>
+  <si>
+    <t>Chocolate Bombs</t>
+  </si>
+  <si>
+    <t>Whistling Rockets</t>
+  </si>
+  <si>
+    <t>Snake Tablets</t>
+  </si>
+  <si>
+    <t>Colourful Sparklers</t>
+  </si>
+  <si>
+    <t>Thunder Bombs</t>
+  </si>
+  <si>
+    <t>Multi-colour Rockets</t>
+  </si>
+  <si>
+    <t>Fountain Crackers</t>
+  </si>
+  <si>
+    <t>Disco Lights</t>
+  </si>
+  <si>
+    <t>Garland Crackers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,10 +152,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,65 +474,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742260DC-49AE-4DD8-A04F-9EBE2A1331A7}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>100</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>200</v>
+      </c>
+      <c r="B3" s="1">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>100</v>
-      </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>150</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>180</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>130</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>210</v>
+      </c>
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>90</v>
+      </c>
+      <c r="B8" s="1">
         <v>50</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>220</v>
+      </c>
+      <c r="B9" s="1">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>160</v>
+      </c>
+      <c r="B10" s="1">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>200</v>
       </c>
-      <c r="C3" s="1">
+      <c r="B11" s="1">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>110</v>
+      </c>
+      <c r="B12" s="1">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>175</v>
+      </c>
+      <c r="B13" s="1">
         <v>30</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>140</v>
+      </c>
+      <c r="B14" s="1">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>190</v>
+      </c>
+      <c r="B15" s="1">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>160</v>
+      </c>
+      <c r="B16" s="1">
+        <v>80</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>210</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>120</v>
+      </c>
+      <c r="B18" s="1">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>180</v>
+      </c>
+      <c r="B19" s="1">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>220</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1">
+        <v>110</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>